<commit_message>
Se agrega nueva notebook con random search y LightGBM, otra para probar las predicciones. Se puede parametrizar estrategia de entrenamiento, se completa historia desde primera aparicion de producto y se filtran los productos a predecir
</commit_message>
<xml_diff>
--- a/docs/DecisionesTomadas.xlsx
+++ b/docs/DecisionesTomadas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_MCD\_Labo3\code\labo3_empresa3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911F35A3-3ACE-4C1E-B69D-59A1E8A746A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091245AC-5A68-42CE-B1DD-B2DC89EC0A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1755" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Duplicaciones y faltantes en Maestro de Productos</t>
   </si>
@@ -44,6 +44,16 @@
   <si>
     <t xml:space="preserve"> - Se encontraron productos con múltiples cat3 (20623 y 20230), se les dejó solamente una (SHAMPOO, según su brand SHAMPOO3)
  - 13 productos no tenían cat1, se les asignó FOOD (eran TE)</t>
+  </si>
+  <si>
+    <t>Predicción de Productos</t>
+  </si>
+  <si>
+    <t>Predicción</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - No se predicen productos discontinuados (sin ventas en 201904,201905,201906)
+ - No se predicen productos con menos de 3 meses de historia (aparecidos despúes en 201902 o más)</t>
   </si>
 </sst>
 </file>
@@ -108,7 +118,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -119,6 +129,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -403,7 +416,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,10 +448,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>

</xml_diff>